<commit_message>
Updated Day1 and added notes to day2
</commit_message>
<xml_diff>
--- a/assignment8/src/MeetingNotes/Daily Scrum - Meeting Notes.xlsx
+++ b/assignment8/src/MeetingNotes/Daily Scrum - Meeting Notes.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Google Drive Unlimiteddigits\IPFW\2016 Fall\Essentials of Software engineering\Assignments\assignment-8\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16455" windowHeight="7065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14190" windowHeight="5505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Day (1)" sheetId="1" r:id="rId1"/>
@@ -29,6 +24,7 @@
     <sheet name="Day (15)" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1:M16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="27">
   <si>
     <t>Daily Scrum Meeting (e-version)</t>
   </si>
@@ -92,6 +88,38 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Mark Erickson</t>
+  </si>
+  <si>
+    <t>Created List of questions to ask customer</t>
+  </si>
+  <si>
+    <t>Add more to the Sprint Backlog</t>
+  </si>
+  <si>
+    <t>Reviewed online calculator</t>
+  </si>
+  <si>
+    <t>Test Main.java</t>
+  </si>
+  <si>
+    <t>created Sprint Planning Meeting Notes</t>
+  </si>
+  <si>
+    <t>Aaron Elliott</t>
+  </si>
+  <si>
+    <t>Created link and repositiory in GitHub.
+Rewatched GitHub checkout video
+Established two workstations (laptops) for testing.  One to do the initial push and commit to GitHub, the other successfully checked out the code remotely and did a successful commit and push.
+Installed and worked/learned Windows Builder for Eclipse.</t>
+  </si>
+  <si>
+    <t>Answer product questions for client
+Will look into understanding Scrum Master duties
+Start on chapter review questions</t>
   </si>
 </sst>
 </file>
@@ -250,13 +278,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -293,7 +319,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:I5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,20 +639,20 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <v>42670</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -620,21 +663,21 @@
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="6"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -711,22 +754,22 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
@@ -735,27 +778,31 @@
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
+    <row r="13" spans="1:9" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="18"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
@@ -802,15 +849,15 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -826,13 +873,13 @@
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -894,24 +941,20 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="G23:I23"/>
     <mergeCell ref="G24:I24"/>
     <mergeCell ref="G25:I25"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="D23:F23"/>
     <mergeCell ref="D24:F24"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="A13:C13"/>
@@ -924,9 +967,10 @@
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
@@ -942,6 +986,9 @@
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -972,46 +1019,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (9)'!H1+1</f>
         <v>42679</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -1072,37 +1119,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -1163,37 +1210,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -1255,54 +1302,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1332,46 +1379,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (10)'!H1+1</f>
         <v>42680</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -1432,37 +1479,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -1523,37 +1570,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -1633,18 +1680,24 @@
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="A16:C16"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:I14"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:I8"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
     <mergeCell ref="A5:C5"/>
@@ -1652,17 +1705,11 @@
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1692,46 +1739,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (11)'!H1+1</f>
         <v>42681</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -1792,37 +1839,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -1883,37 +1930,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -1975,54 +2022,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2052,46 +2099,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (12)'!H1+1</f>
         <v>42682</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -2152,37 +2199,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -2243,37 +2290,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -2335,54 +2382,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2412,46 +2459,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (13)'!H1+1</f>
         <v>42683</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -2512,37 +2559,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -2603,37 +2650,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -2695,54 +2742,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2772,46 +2819,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (14)'!H1+1</f>
         <v>42684</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -2872,37 +2919,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -2963,37 +3010,407 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="12"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="12"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="12"/>
+    </row>
+    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3">
+        <f>'Day (1)'!H1+1</f>
+        <v>42671</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="15"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -3073,6 +3490,7 @@
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
@@ -3085,384 +3503,23 @@
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="16">
-        <f>'Day (1)'!H1+1</f>
-        <v>42671</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="12"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="12"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="12"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="12"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="12"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="12"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="12"/>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3492,46 +3549,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (2)'!H1+1</f>
         <v>42672</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -3592,37 +3649,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -3683,37 +3740,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -3775,54 +3832,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3852,46 +3909,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (3)'!H1+1</f>
         <v>42673</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -3952,37 +4009,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -4043,37 +4100,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -4135,54 +4192,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4212,46 +4269,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (4)'!H1+1</f>
         <v>42674</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -4312,37 +4369,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -4403,37 +4460,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -4495,54 +4552,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4572,46 +4629,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (5)'!H1+1</f>
         <v>42675</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -4672,37 +4729,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -4763,37 +4820,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -4855,54 +4912,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4932,46 +4989,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (6)'!H1+1</f>
         <v>42676</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -5032,37 +5089,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -5123,37 +5180,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -5215,54 +5272,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5292,46 +5349,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (7)'!H1+1</f>
         <v>42677</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -5392,37 +5449,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -5483,37 +5540,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -5575,54 +5632,54 @@
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="G23:I23"/>
     <mergeCell ref="A24:C24"/>
     <mergeCell ref="D24:F24"/>
     <mergeCell ref="G24:I24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:I14"/>
     <mergeCell ref="A15:C15"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5652,46 +5709,46 @@
       <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="16">
+      <c r="H1" s="3">
         <f>'Day (8)'!H1+1</f>
         <v>42678</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" t="s">
         <v>3</v>
       </c>
@@ -5752,37 +5809,37 @@
       <c r="I9" s="15"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" t="s">
         <v>3</v>
       </c>
@@ -5843,37 +5900,37 @@
       <c r="I17" s="15"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
       <c r="D20" t="s">
         <v>2</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -5950,9 +6007,6 @@
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="D22:F22"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="D17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
@@ -5965,24 +6019,27 @@
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:F8"/>
     <mergeCell ref="G8:I8"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="D9:F9"/>
     <mergeCell ref="G9:I9"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated day 7 and 8
</commit_message>
<xml_diff>
--- a/assignment8/src/MeetingNotes/Daily Scrum - Meeting Notes.xlsx
+++ b/assignment8/src/MeetingNotes/Daily Scrum - Meeting Notes.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\git12\assignment8\src\MeetingNotes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8280" windowHeight="2970" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="4710" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Day (1)" sheetId="1" r:id="rId1"/>
@@ -29,6 +24,7 @@
     <sheet name="Day (15)" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1:T13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="72">
   <si>
     <t>Daily Scrum Meeting (e-version)</t>
   </si>
@@ -247,6 +243,18 @@
   </si>
   <si>
     <t>Will correspond with group for preparations for Sprint 1 review.</t>
+  </si>
+  <si>
+    <t>Prepare and particpate in Sprint 1 review.</t>
+  </si>
+  <si>
+    <t>Sprint 2 planning</t>
+  </si>
+  <si>
+    <t>Disabled visibility for  distance textfield and combobox for kilometers and miles.</t>
+  </si>
+  <si>
+    <t>Updated code to do checks for invalid user input.</t>
   </si>
 </sst>
 </file>
@@ -4822,7 +4830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D13" sqref="D13:F13"/>
     </sheetView>
   </sheetViews>
@@ -5186,8 +5194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5321,7 +5329,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -5342,26 +5350,30 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
+      <c r="A13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -5539,6 +5551,7 @@
     <mergeCell ref="G24:I24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5547,7 +5560,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D13" sqref="D13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5681,7 +5694,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
@@ -5701,27 +5714,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
+    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="24"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>

</xml_diff>

<commit_message>
Updated Daily scrum meeting notes
</commit_message>
<xml_diff>
--- a/assignment8/src/MeetingNotes/Daily Scrum - Meeting Notes.xlsx
+++ b/assignment8/src/MeetingNotes/Daily Scrum - Meeting Notes.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\git12\assignment8\src\MeetingNotes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="4710" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15600" windowHeight="4710" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Day (1)" sheetId="1" r:id="rId1"/>
@@ -28,9 +23,9 @@
     <sheet name="Day (14)" sheetId="15" r:id="rId14"/>
     <sheet name="Day (15)" sheetId="16" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -38,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="84">
   <si>
     <t>Daily Scrum Meeting (e-version)</t>
   </si>
@@ -260,12 +255,48 @@
   <si>
     <t>Updated code to do checks for invalid user input.</t>
   </si>
+  <si>
+    <t>removed hungarian notation</t>
+  </si>
+  <si>
+    <t>Created burndown chart</t>
+  </si>
+  <si>
+    <t>Added test cases provided by client</t>
+  </si>
+  <si>
+    <t>review math formulas</t>
+  </si>
+  <si>
+    <t>Try to get PaceCalculator to work with window builder</t>
+  </si>
+  <si>
+    <t>rename version that doesn't work</t>
+  </si>
+  <si>
+    <t>Renamed PaceCalculator that didn't have design tab</t>
+  </si>
+  <si>
+    <t>Add some limits to the input fields then merge them if someone has made changes to PaceCalculator</t>
+  </si>
+  <si>
+    <t>Refine Backlogs and burndown chart from class discussion</t>
+  </si>
+  <si>
+    <t>Had computer difficulties</t>
+  </si>
+  <si>
+    <t>Copied functionality from V1 to new PaceCalculator</t>
+  </si>
+  <si>
+    <t>Review checkstyle &amp; PaceCalculator</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -485,6 +516,24 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +594,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -580,7 +629,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,21 +806,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="G22" sqref="G22:I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
@@ -780,7 +829,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -791,7 +840,7 @@
         <v>42670</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -802,7 +851,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -815,7 +864,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -830,7 +879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
@@ -847,7 +896,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -862,7 +911,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10" t="s">
         <v>11</v>
       </c>
@@ -877,7 +926,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -890,7 +939,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -901,7 +950,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -912,7 +961,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -922,7 +971,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -937,7 +986,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="160.5" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>25</v>
       </c>
@@ -952,7 +1001,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -963,7 +1012,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -974,7 +1023,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -985,7 +1034,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -996,7 +1045,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1007,7 +1056,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1066,7 @@
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1032,7 +1081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
         <v>42</v>
       </c>
@@ -1049,7 +1098,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10" t="s">
         <v>43</v>
       </c>
@@ -1064,7 +1113,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -1077,7 +1126,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -1088,7 +1137,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -1156,14 +1205,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -1172,7 +1221,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1184,7 +1233,7 @@
         <v>42679</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1195,7 +1244,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1208,7 +1257,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1223,29 +1272,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:9">
+      <c r="A5" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -1256,7 +1309,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -1267,7 +1320,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -1278,7 +1331,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1289,7 +1342,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1299,7 +1352,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1314,7 +1367,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -1325,7 +1378,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -1336,7 +1389,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -1347,7 +1400,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -1358,7 +1411,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -1369,7 +1422,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1380,7 +1433,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1390,7 +1443,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1405,7 +1458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -1416,7 +1469,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -1427,7 +1480,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -1438,7 +1491,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -1449,7 +1502,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -1461,7 +1514,7 @@
       <c r="I25" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="47">
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -1499,15 +1552,14 @@
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D5:F6"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:F8"/>
   </mergeCells>
@@ -1516,14 +1568,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -1532,7 +1584,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1596,7 @@
         <v>42680</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1555,7 +1607,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1568,7 +1620,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1583,7 +1635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -1594,7 +1646,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -1605,7 +1657,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -1616,7 +1668,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -1627,7 +1679,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -1638,7 +1690,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1649,7 +1701,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -1659,7 +1711,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1674,7 +1726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -1685,7 +1737,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -1696,7 +1748,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -1707,7 +1759,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -1718,7 +1770,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -1729,7 +1781,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1740,7 +1792,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -1750,7 +1802,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1765,7 +1817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -1776,7 +1828,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -1787,7 +1839,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -1798,7 +1850,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -1809,7 +1861,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -1876,14 +1928,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -1892,7 +1944,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1904,7 +1956,7 @@
         <v>42681</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1915,7 +1967,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1928,7 +1980,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1943,7 +1995,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -1954,7 +2006,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -1965,7 +2017,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -1976,7 +2028,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -1987,7 +2039,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -1998,7 +2050,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2009,7 +2061,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2019,7 +2071,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2034,7 +2086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -2045,7 +2097,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -2056,7 +2108,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -2067,7 +2119,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -2078,7 +2130,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -2089,7 +2141,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2100,7 +2152,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -2110,7 +2162,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2125,7 +2177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -2136,7 +2188,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -2147,7 +2199,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -2158,7 +2210,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -2169,7 +2221,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -2236,14 +2288,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -2252,7 +2304,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2264,7 +2316,7 @@
         <v>42682</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2275,7 +2327,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2288,7 +2340,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2303,7 +2355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -2314,7 +2366,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2325,7 +2377,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -2336,7 +2388,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -2347,7 +2399,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -2358,7 +2410,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2369,7 +2421,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2379,7 +2431,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2394,7 +2446,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -2405,7 +2457,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -2416,7 +2468,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -2427,7 +2479,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -2438,7 +2490,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -2449,7 +2501,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2460,7 +2512,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -2470,7 +2522,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2485,7 +2537,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -2496,7 +2548,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -2507,7 +2559,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -2518,7 +2570,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -2529,7 +2581,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -2596,14 +2648,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -2612,7 +2664,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2624,7 +2676,7 @@
         <v>42683</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2635,7 +2687,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -2648,7 +2700,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2663,7 +2715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -2674,7 +2726,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -2685,7 +2737,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -2696,7 +2748,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -2707,7 +2759,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -2718,7 +2770,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2729,7 +2781,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2739,7 +2791,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -2754,7 +2806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -2765,7 +2817,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -2776,7 +2828,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -2787,7 +2839,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -2798,7 +2850,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -2809,7 +2861,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -2820,7 +2872,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -2830,7 +2882,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2845,7 +2897,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -2856,7 +2908,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -2867,7 +2919,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -2878,7 +2930,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -2889,7 +2941,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -2956,14 +3008,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -2972,7 +3024,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2984,7 +3036,7 @@
         <v>42684</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2995,7 +3047,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3008,7 +3060,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3023,7 +3075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
@@ -3034,7 +3086,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -3045,7 +3097,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -3056,7 +3108,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -3067,7 +3119,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -3078,7 +3130,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3089,7 +3141,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3099,7 +3151,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3114,7 +3166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -3125,7 +3177,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -3136,7 +3188,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -3147,7 +3199,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -3158,7 +3210,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -3169,7 +3221,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3180,7 +3232,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -3190,7 +3242,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3205,7 +3257,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -3216,7 +3268,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -3227,7 +3279,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -3238,7 +3290,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -3249,7 +3301,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -3316,14 +3368,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23:F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -3332,7 +3384,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3344,7 +3396,7 @@
         <v>42671</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3355,7 +3407,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3368,7 +3420,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3383,7 +3435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>19</v>
       </c>
@@ -3398,7 +3450,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10" t="s">
         <v>21</v>
       </c>
@@ -3413,7 +3465,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10" t="s">
         <v>23</v>
       </c>
@@ -3426,7 +3478,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -3437,7 +3489,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -3448,7 +3500,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3459,7 +3511,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3469,7 +3521,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3484,7 +3536,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="41.25" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
@@ -3499,7 +3551,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="22" t="s">
         <v>29</v>
       </c>
@@ -3512,7 +3564,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
@@ -3523,7 +3575,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="22"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
@@ -3534,7 +3586,7 @@
       <c r="H16" s="23"/>
       <c r="I16" s="24"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -3545,7 +3597,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3556,7 +3608,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -3566,7 +3618,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3581,7 +3633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
         <v>48</v>
       </c>
@@ -3596,7 +3648,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10" t="s">
         <v>49</v>
       </c>
@@ -3611,7 +3663,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10" t="s">
         <v>50</v>
       </c>
@@ -3624,7 +3676,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -3635,7 +3687,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -3703,14 +3755,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
@@ -3719,7 +3771,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3731,7 +3783,7 @@
         <v>42672</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3742,7 +3794,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -3755,7 +3807,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3770,7 +3822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>36</v>
       </c>
@@ -3785,7 +3837,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10" t="s">
         <v>38</v>
       </c>
@@ -3800,7 +3852,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10" t="s">
         <v>40</v>
       </c>
@@ -3813,7 +3865,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -3824,7 +3876,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -3835,7 +3887,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -3846,7 +3898,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -3856,7 +3908,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -3871,7 +3923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>31</v>
       </c>
@@ -3886,7 +3938,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -3897,7 +3949,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="22"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
@@ -3908,7 +3960,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -3919,7 +3971,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -3930,7 +3982,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -3941,7 +3993,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -3951,7 +4003,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -3966,7 +4018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
         <v>53</v>
       </c>
@@ -3981,7 +4033,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10" t="s">
         <v>54</v>
       </c>
@@ -3994,7 +4046,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -4005,7 +4057,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -4016,7 +4068,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -4084,14 +4136,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -4100,7 +4152,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4112,7 +4164,7 @@
         <v>42673</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4123,7 +4175,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4136,7 +4188,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4151,7 +4203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>58</v>
       </c>
@@ -4166,7 +4218,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -4177,7 +4229,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -4188,7 +4240,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -4199,7 +4251,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -4210,7 +4262,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4221,7 +4273,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4231,7 +4283,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -4246,7 +4298,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="66" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>33</v>
       </c>
@@ -4263,7 +4315,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -4274,7 +4326,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -4285,7 +4337,7 @@
       <c r="H15" s="23"/>
       <c r="I15" s="24"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -4296,7 +4348,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -4307,7 +4359,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4318,7 +4370,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -4328,7 +4380,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -4343,7 +4395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7" t="s">
         <v>56</v>
       </c>
@@ -4358,7 +4410,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -4369,7 +4421,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -4380,7 +4432,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -4391,7 +4443,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -4458,14 +4510,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -4474,7 +4526,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4486,7 +4538,7 @@
         <v>42674</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4497,7 +4549,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -4510,7 +4562,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4525,7 +4577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="7" t="s">
         <v>60</v>
       </c>
@@ -4540,7 +4592,7 @@
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
@@ -4553,7 +4605,7 @@
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -4564,7 +4616,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -4575,7 +4627,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -4586,7 +4638,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4597,7 +4649,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4607,7 +4659,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -4622,7 +4674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="96" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>63</v>
       </c>
@@ -4639,7 +4691,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -4650,7 +4702,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -4661,7 +4713,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -4672,7 +4724,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -4683,7 +4735,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -4694,7 +4746,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -4704,7 +4756,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -4719,7 +4771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -4730,7 +4782,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -4741,7 +4793,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -4752,7 +4804,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -4763,7 +4815,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -4831,14 +4883,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -4847,7 +4899,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4859,7 +4911,7 @@
         <v>42675</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4870,12 +4922,12 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -4883,7 +4935,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -4898,29 +4950,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:9">
+      <c r="A5" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10" t="s">
+        <v>74</v>
+      </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -4931,7 +4991,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -4942,7 +5002,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -4953,7 +5013,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -4964,7 +5024,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -4974,7 +5034,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -4989,7 +5049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="72.75" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>66</v>
       </c>
@@ -5004,7 +5064,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -5015,7 +5075,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -5026,7 +5086,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -5037,7 +5097,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -5048,7 +5108,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5059,7 +5119,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -5069,7 +5129,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -5084,7 +5144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -5095,7 +5155,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -5106,7 +5166,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -5117,7 +5177,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -5128,7 +5188,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -5195,14 +5255,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -5211,7 +5271,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5223,7 +5283,7 @@
         <v>42676</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5234,12 +5294,12 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -5247,7 +5307,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5262,29 +5322,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:9" ht="30.75" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
+    <row r="6" spans="1:9">
+      <c r="A6" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="12"/>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
@@ -5295,7 +5363,7 @@
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -5306,7 +5374,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -5317,7 +5385,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -5328,7 +5396,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -5338,7 +5406,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -5353,7 +5421,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="28.5" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>68</v>
       </c>
@@ -5368,7 +5436,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="22"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
@@ -5379,7 +5447,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -5390,7 +5458,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -5401,7 +5469,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -5412,7 +5480,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5423,7 +5491,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -5433,7 +5501,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -5448,7 +5516,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -5459,7 +5527,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -5470,7 +5538,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -5481,7 +5549,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -5492,7 +5560,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -5560,14 +5628,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
@@ -5576,7 +5644,7 @@
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5588,7 +5656,7 @@
         <v>42677</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5599,12 +5667,12 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -5612,7 +5680,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5627,43 +5695,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+    <row r="5" spans="1:9" ht="39" customHeight="1">
+      <c r="A5" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
+    <row r="6" spans="1:9" ht="33" customHeight="1">
+      <c r="A6" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
+    <row r="7" spans="1:9">
+      <c r="A7" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
+    <row r="8" spans="1:9">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
       <c r="F8" s="12"/>
@@ -5671,7 +5749,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -5682,7 +5760,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -5693,7 +5771,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -5703,7 +5781,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -5718,7 +5796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="30" customHeight="1">
       <c r="A13" s="16" t="s">
         <v>69</v>
       </c>
@@ -5733,7 +5811,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="48" customHeight="1">
       <c r="A14" s="22" t="s">
         <v>70</v>
       </c>
@@ -5746,7 +5824,7 @@
       <c r="H14" s="23"/>
       <c r="I14" s="24"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -5757,7 +5835,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -5768,7 +5846,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -5779,7 +5857,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -5790,7 +5868,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -5800,7 +5878,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -5815,7 +5893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -5826,7 +5904,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -5837,7 +5915,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -5848,7 +5926,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -5859,7 +5937,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -5871,7 +5949,7 @@
       <c r="I25" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="47">
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -5907,6 +5985,7 @@
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:F13"/>
     <mergeCell ref="G13:I13"/>
+    <mergeCell ref="A7:C8"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:F6"/>
@@ -5914,11 +5993,9 @@
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="A7:C7"/>
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5926,23 +6003,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D5" sqref="D5:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5954,7 +6031,7 @@
         <v>42678</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -5965,12 +6042,12 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="21"/>
       <c r="D3" s="21"/>
@@ -5978,7 +6055,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -5993,40 +6070,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:9" ht="15" customHeight="1">
+      <c r="A5" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" thickBot="1">
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
       <c r="I6" s="12"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
+    <row r="7" spans="1:9">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
       <c r="I7" s="12"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
@@ -6037,7 +6118,7 @@
       <c r="H8" s="11"/>
       <c r="I8" s="12"/>
     </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -6048,7 +6129,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="15"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -6059,7 +6140,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -6069,7 +6150,7 @@
       <c r="C11" s="21"/>
       <c r="D11" s="21"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -6084,7 +6165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
@@ -6095,7 +6176,7 @@
       <c r="H13" s="8"/>
       <c r="I13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -6106,7 +6187,7 @@
       <c r="H14" s="11"/>
       <c r="I14" s="12"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -6117,7 +6198,7 @@
       <c r="H15" s="11"/>
       <c r="I15" s="12"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -6128,7 +6209,7 @@
       <c r="H16" s="11"/>
       <c r="I16" s="12"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15.75" thickBot="1">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="15"/>
@@ -6139,7 +6220,7 @@
       <c r="H17" s="14"/>
       <c r="I17" s="15"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -6150,7 +6231,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -6160,7 +6241,7 @@
       <c r="C19" s="21"/>
       <c r="D19" s="21"/>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15.75" thickBot="1">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -6175,7 +6256,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
@@ -6186,7 +6267,7 @@
       <c r="H21" s="8"/>
       <c r="I21" s="9"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
@@ -6197,7 +6278,7 @@
       <c r="H22" s="11"/>
       <c r="I22" s="12"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
@@ -6208,7 +6289,7 @@
       <c r="H23" s="11"/>
       <c r="I23" s="12"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
@@ -6219,7 +6300,7 @@
       <c r="H24" s="11"/>
       <c r="I24" s="12"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15.75" thickBot="1">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
@@ -6231,7 +6312,7 @@
       <c r="I25" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
+  <mergeCells count="46">
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="D25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -6267,16 +6348,14 @@
     <mergeCell ref="G16:I16"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D5:F7"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:F5"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="D8:F8"/>
     <mergeCell ref="D17:F17"/>

</xml_diff>